<commit_message>
corrections to modular paths
</commit_message>
<xml_diff>
--- a/medea/data/processed/plant-list_hydro.xlsx
+++ b/medea/data/processed/plant-list_hydro.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea_open\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\medea_PolicyAustria\medea\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C5A4B6-3022-49DD-AE57-EF006A051413}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCE53F50-326B-4DE1-A864-F9CC5581FF7F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opsd_hydro" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2562" uniqueCount="874">
   <si>
     <t>company</t>
   </si>
@@ -2674,6 +2674,21 @@
   </si>
   <si>
     <t>https://de.wikipedia.org/wiki/Pumpspeicherkraftwerk_Waldeck#Waldeck_II</t>
+  </si>
+  <si>
+    <t>energy_max</t>
+  </si>
+  <si>
+    <t>power_in</t>
+  </si>
+  <si>
+    <t>power_out</t>
+  </si>
+  <si>
+    <t>efficiency_out</t>
+  </si>
+  <si>
+    <t>efficiency_in</t>
   </si>
 </sst>
 </file>
@@ -3158,9 +3173,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AK229"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I229" sqref="I229"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3195,7 +3210,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>724</v>
+        <v>871</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -3252,13 +3267,13 @@
         <v>20</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>726</v>
+        <v>869</v>
       </c>
       <c r="AA1" t="s">
         <v>21</v>
       </c>
       <c r="AB1" t="s">
-        <v>725</v>
+        <v>870</v>
       </c>
       <c r="AC1" t="s">
         <v>691</v>
@@ -3267,10 +3282,10 @@
         <v>723</v>
       </c>
       <c r="AE1" t="s">
-        <v>727</v>
+        <v>872</v>
       </c>
       <c r="AF1" t="s">
-        <v>728</v>
+        <v>873</v>
       </c>
       <c r="AG1" t="s">
         <v>695</v>
@@ -17548,15 +17563,15 @@
         <v>21.679292929292931</v>
       </c>
       <c r="AD200">
-        <f>ROUND(0.95*IF($T200="Pelton",0.875,IF($T200="Kaplan",0.9,0.925))*IF($I200="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" ref="AD200:AD229" si="31">ROUND(0.95*IF($T200="Pelton",0.875,IF($T200="Kaplan",0.9,0.925))*IF($I200="Pumped Storage",0.875,1),2)</f>
         <v>0.88</v>
       </c>
       <c r="AE200">
-        <f t="shared" ref="AE200:AE229" si="31">ROUND(SQRT($AD200),3)*0.975</f>
+        <f t="shared" ref="AE200:AE229" si="32">ROUND(SQRT($AD200),3)*0.975</f>
         <v>0.91454999999999997</v>
       </c>
       <c r="AF200">
-        <f t="shared" ref="AF200:AF229" si="32">ROUND(SQRT($AD200),3)*1.025</f>
+        <f t="shared" ref="AF200:AF229" si="33">ROUND(SQRT($AD200),3)*1.025</f>
         <v>0.9614499999999998</v>
       </c>
     </row>
@@ -17634,15 +17649,15 @@
         <v>25</v>
       </c>
       <c r="AD201">
-        <f>ROUND(0.95*IF($T201="Pelton",0.875,IF($T201="Kaplan",0.9,0.925))*IF($I201="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE201">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF201">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -17708,15 +17723,15 @@
         <v>200</v>
       </c>
       <c r="AD202">
-        <f>ROUND(0.95*IF($T202="Pelton",0.875,IF($T202="Kaplan",0.9,0.925))*IF($I202="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE202">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF202">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -17791,15 +17806,15 @@
         <v>99</v>
       </c>
       <c r="AD203">
-        <f>ROUND(0.95*IF($T203="Pelton",0.875,IF($T203="Kaplan",0.9,0.925))*IF($I203="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE203">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF203">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -17874,15 +17889,15 @@
         <v>320</v>
       </c>
       <c r="AD204">
-        <f>ROUND(0.95*IF($T204="Pelton",0.875,IF($T204="Kaplan",0.9,0.925))*IF($I204="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE204">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF204">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -17948,15 +17963,15 @@
         <v>0.9</v>
       </c>
       <c r="AD205">
-        <f>ROUND(0.95*IF($T205="Pelton",0.875,IF($T205="Kaplan",0.9,0.925))*IF($I205="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE205">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF205">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18028,15 +18043,15 @@
         <v>40</v>
       </c>
       <c r="AD206">
-        <f>ROUND(0.95*IF($T206="Pelton",0.875,IF($T206="Kaplan",0.9,0.925))*IF($I206="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE206">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF206">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18081,15 +18096,15 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AD207">
-        <f>ROUND(0.95*IF($T207="Pelton",0.875,IF($T207="Kaplan",0.9,0.925))*IF($I207="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.88</v>
       </c>
       <c r="AE207">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.91454999999999997</v>
       </c>
       <c r="AF207">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.9614499999999998</v>
       </c>
     </row>
@@ -18161,15 +18176,15 @@
         <v>26</v>
       </c>
       <c r="AD208">
-        <f>ROUND(0.95*IF($T208="Pelton",0.875,IF($T208="Kaplan",0.9,0.925))*IF($I208="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE208">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF208">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18244,15 +18259,15 @@
         <v>88.8</v>
       </c>
       <c r="AD209">
-        <f>ROUND(0.95*IF($T209="Pelton",0.875,IF($T209="Kaplan",0.9,0.925))*IF($I209="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE209">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF209">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18321,15 +18336,15 @@
         <v>102</v>
       </c>
       <c r="AD210">
-        <f>ROUND(0.95*IF($T210="Pelton",0.875,IF($T210="Kaplan",0.9,0.925))*IF($I210="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE210">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF210">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18404,15 +18419,15 @@
         <v>40</v>
       </c>
       <c r="AD211">
-        <f>ROUND(0.95*IF($T211="Pelton",0.875,IF($T211="Kaplan",0.9,0.925))*IF($I211="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE211">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF211">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18481,15 +18496,15 @@
         <v>84</v>
       </c>
       <c r="AD212">
-        <f>ROUND(0.95*IF($T212="Pelton",0.875,IF($T212="Kaplan",0.9,0.925))*IF($I212="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE212">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF212">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18552,15 +18567,15 @@
         <v>25</v>
       </c>
       <c r="AD213">
-        <f>ROUND(0.95*IF($T213="Pelton",0.875,IF($T213="Kaplan",0.9,0.925))*IF($I213="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE213">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF213">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18626,15 +18641,15 @@
         <v>45.4</v>
       </c>
       <c r="AD214">
-        <f>ROUND(0.95*IF($T214="Pelton",0.875,IF($T214="Kaplan",0.9,0.925))*IF($I214="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE214">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF214">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18700,15 +18715,15 @@
         <v>36.799999999999997</v>
       </c>
       <c r="AD215">
-        <f>ROUND(0.95*IF($T215="Pelton",0.875,IF($T215="Kaplan",0.9,0.925))*IF($I215="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE215">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF215">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18783,15 +18798,15 @@
         <v>60</v>
       </c>
       <c r="AD216">
-        <f>ROUND(0.95*IF($T216="Pelton",0.875,IF($T216="Kaplan",0.9,0.925))*IF($I216="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE216">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF216">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18866,15 +18881,15 @@
         <v>66</v>
       </c>
       <c r="AD217">
-        <f>ROUND(0.95*IF($T217="Pelton",0.875,IF($T217="Kaplan",0.9,0.925))*IF($I217="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE217">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF217">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -18937,15 +18952,15 @@
         <v>154</v>
       </c>
       <c r="AD218">
-        <f>ROUND(0.95*IF($T218="Pelton",0.875,IF($T218="Kaplan",0.9,0.925))*IF($I218="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE218">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF218">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -19017,15 +19032,15 @@
         <v>20</v>
       </c>
       <c r="AD219">
-        <f>ROUND(0.95*IF($T219="Pelton",0.875,IF($T219="Kaplan",0.9,0.925))*IF($I219="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE219">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF219">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -19091,15 +19106,15 @@
         <v>140</v>
       </c>
       <c r="AD220">
-        <f>ROUND(0.95*IF($T220="Pelton",0.875,IF($T220="Kaplan",0.9,0.925))*IF($I220="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE220">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF220">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -19171,15 +19186,15 @@
         <v>0</v>
       </c>
       <c r="AD221">
-        <f>ROUND(0.95*IF($T221="Pelton",0.875,IF($T221="Kaplan",0.9,0.925))*IF($I221="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.86</v>
       </c>
       <c r="AE221">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.90382499999999999</v>
       </c>
       <c r="AF221">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.95017499999999999</v>
       </c>
     </row>
@@ -19248,15 +19263,15 @@
         <v>22</v>
       </c>
       <c r="AD222">
-        <f>ROUND(0.95*IF($T222="Pelton",0.875,IF($T222="Kaplan",0.9,0.925))*IF($I222="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.73</v>
       </c>
       <c r="AE222">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.83265</v>
       </c>
       <c r="AF222">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.87534999999999985</v>
       </c>
     </row>
@@ -19331,15 +19346,15 @@
         <v>67</v>
       </c>
       <c r="AD223">
-        <f>ROUND(0.95*IF($T223="Pelton",0.875,IF($T223="Kaplan",0.9,0.925))*IF($I223="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE223">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF223">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -19411,15 +19426,15 @@
         <v>0</v>
       </c>
       <c r="AD224">
-        <f>ROUND(0.95*IF($T224="Pelton",0.875,IF($T224="Kaplan",0.9,0.925))*IF($I224="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.88</v>
       </c>
       <c r="AE224">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.91454999999999997</v>
       </c>
       <c r="AF224">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.9614499999999998</v>
       </c>
     </row>
@@ -19485,15 +19500,15 @@
         <v>480</v>
       </c>
       <c r="AD225">
-        <f>ROUND(0.95*IF($T225="Pelton",0.875,IF($T225="Kaplan",0.9,0.925))*IF($I225="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE225">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF225">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -19559,15 +19574,15 @@
         <v>140</v>
       </c>
       <c r="AD226">
-        <f>ROUND(0.95*IF($T226="Pelton",0.875,IF($T226="Kaplan",0.9,0.925))*IF($I226="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE226">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF226">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -19639,15 +19654,15 @@
         <v>144</v>
       </c>
       <c r="AD227">
-        <f>ROUND(0.95*IF($T227="Pelton",0.875,IF($T227="Kaplan",0.9,0.925))*IF($I227="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE227">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF227">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -19722,15 +19737,15 @@
         <v>52</v>
       </c>
       <c r="AD228">
-        <f>ROUND(0.95*IF($T228="Pelton",0.875,IF($T228="Kaplan",0.9,0.925))*IF($I228="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE228">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF228">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>
@@ -19805,15 +19820,15 @@
         <v>40</v>
       </c>
       <c r="AD229">
-        <f>ROUND(0.95*IF($T229="Pelton",0.875,IF($T229="Kaplan",0.9,0.925))*IF($I229="Pumped Storage",0.875,1),2)</f>
+        <f t="shared" si="31"/>
         <v>0.77</v>
       </c>
       <c r="AE229">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>0.85507500000000003</v>
       </c>
       <c r="AF229">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>0.89892499999999997</v>
       </c>
     </row>

</xml_diff>